<commit_message>
Documento de arquitetura e plano de desenvolvimento
</commit_message>
<xml_diff>
--- a/docs/Comissão Smart, consultores e operadores.xlsx
+++ b/docs/Comissão Smart, consultores e operadores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\OneDrive\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\11-git-rodrigobaia\smart-consultoria-system\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCFBF01-8F90-44FF-928B-5678E37F8871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D424F1-87C8-45E1-9585-AA399ED2E993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EC3DB532-1D1E-47D1-84C6-B60AFB32DD99}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{EC3DB532-1D1E-47D1-84C6-B60AFB32DD99}"/>
   </bookViews>
   <sheets>
     <sheet name="Lojas Leves" sheetId="3" r:id="rId1"/>
@@ -34,6 +34,9 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -560,21 +563,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40A141EC-6F5A-4169-BDD2-0C6D36D69142}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="15.77734375" customWidth="1"/>
-    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -609,7 +617,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -644,7 +652,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -679,7 +687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -714,7 +722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -749,7 +757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="10"/>
@@ -762,7 +770,7 @@
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="10"/>
@@ -775,7 +783,7 @@
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="10"/>
@@ -788,7 +796,7 @@
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="10"/>
@@ -801,7 +809,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="10"/>
@@ -814,7 +822,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="10"/>
@@ -827,7 +835,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="10"/>
@@ -840,7 +848,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="10"/>
@@ -853,7 +861,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="10"/>
@@ -866,7 +874,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="10"/>
@@ -879,7 +887,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="10"/>
@@ -892,7 +900,7 @@
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="10"/>
@@ -905,7 +913,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="10"/>
@@ -918,7 +926,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="10"/>
@@ -931,7 +939,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="10"/>
@@ -944,7 +952,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>14</v>
       </c>
@@ -998,13 +1006,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="16.5546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="16.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="9" t="s">
         <v>3</v>
@@ -1034,7 +1042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -1066,7 +1074,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
@@ -1098,7 +1106,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -1143,17 +1151,17 @@
       <selection activeCell="I2" sqref="I2:I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="15.77734375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="15.77734375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="15.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="15.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1191,7 +1199,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <f>'Lojas Leves'!A2</f>
         <v>1</v>
@@ -1241,7 +1249,7 @@
         <v>11581.775100000001</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <f>'Lojas Leves'!A3</f>
         <v>2</v>
@@ -1291,7 +1299,7 @@
         <v>10431.775100000001</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <f>'Lojas Leves'!A4</f>
         <v>3</v>
@@ -1341,7 +1349,7 @@
         <v>19978</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <f>'Lojas Leves'!A5</f>
         <v>4</v>
@@ -1391,7 +1399,7 @@
         <v>7478</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <f>'Lojas Leves'!A6</f>
         <v>0</v>
@@ -1441,7 +1449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <f>'Lojas Leves'!A7</f>
         <v>0</v>
@@ -1491,7 +1499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <f>'Lojas Leves'!A8</f>
         <v>0</v>
@@ -1541,7 +1549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <f>'Lojas Leves'!A9</f>
         <v>0</v>
@@ -1591,7 +1599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <f>'Lojas Leves'!A10</f>
         <v>0</v>
@@ -1641,7 +1649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <f>'Lojas Leves'!A11</f>
         <v>0</v>
@@ -1691,7 +1699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <f>'Lojas Leves'!A12</f>
         <v>0</v>
@@ -1741,7 +1749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <f>'Lojas Leves'!A13</f>
         <v>0</v>
@@ -1791,7 +1799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <f>'Lojas Leves'!A14</f>
         <v>0</v>
@@ -1841,7 +1849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <f>'Lojas Leves'!A15</f>
         <v>0</v>
@@ -1891,7 +1899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <f>'Lojas Leves'!A16</f>
         <v>0</v>
@@ -1941,7 +1949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <f>'Lojas Leves'!A17</f>
         <v>0</v>
@@ -1991,7 +1999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <f>'Lojas Leves'!A18</f>
         <v>0</v>
@@ -2041,7 +2049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <f>'Lojas Leves'!A19</f>
         <v>0</v>
@@ -2091,7 +2099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <f>'Lojas Leves'!A20</f>
         <v>0</v>
@@ -2141,49 +2149,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C21" s="15">
-        <f>SUM(C2:C20)</f>
+        <f t="shared" ref="C21:L21" si="1">SUM(C2:C20)</f>
         <v>2400</v>
       </c>
       <c r="D21" s="15">
-        <f>SUM(D2:D20)</f>
+        <f t="shared" si="1"/>
         <v>7932.0262000000012</v>
       </c>
       <c r="E21" s="15">
-        <f>SUM(E2:E20)</f>
+        <f t="shared" si="1"/>
         <v>23383.524000000001</v>
       </c>
       <c r="F21" s="15">
-        <f>SUM(F2:F20)</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="G21" s="15">
-        <f>SUM(G2:G20)</f>
+        <f t="shared" si="1"/>
         <v>396</v>
       </c>
       <c r="H21" s="15">
-        <f>SUM(H2:H20)</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="I21" s="15">
-        <f>SUM(I2:I20)</f>
+        <f t="shared" si="1"/>
         <v>158</v>
       </c>
       <c r="J21" s="15">
-        <f>SUM(J2:J20)</f>
+        <f t="shared" si="1"/>
         <v>9900</v>
       </c>
       <c r="K21" s="15">
-        <f>SUM(K2:K20)</f>
+        <f t="shared" si="1"/>
         <v>4900</v>
       </c>
       <c r="L21" s="15">
-        <f>SUM(L2:L20)</f>
+        <f t="shared" si="1"/>
         <v>49469.550199999998</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K23" s="8" t="s">
         <v>20</v>
       </c>
@@ -2192,7 +2200,7 @@
         <v>24734.775099999999</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K24" s="8" t="s">
         <v>21</v>
       </c>
@@ -2215,15 +2223,15 @@
       <selection activeCell="B2" sqref="B2:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="15.77734375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="15.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2261,7 +2269,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <f>'Lojas Leves'!A2</f>
         <v>1</v>
@@ -2311,7 +2319,7 @@
         <v>9626.5950999999986</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <f>'Lojas Leves'!A3</f>
         <v>2</v>
@@ -2361,7 +2369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <f>'Lojas Leves'!A4</f>
         <v>3</v>
@@ -2411,7 +2419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <f>'Lojas Leves'!A5</f>
         <v>4</v>
@@ -2461,7 +2469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <f>'Lojas Leves'!A6</f>
         <v>0</v>
@@ -2511,7 +2519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <f>'Lojas Leves'!A7</f>
         <v>0</v>
@@ -2561,7 +2569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <f>'Lojas Leves'!A8</f>
         <v>0</v>
@@ -2611,7 +2619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <f>'Lojas Leves'!A9</f>
         <v>0</v>
@@ -2661,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <f>'Lojas Leves'!A10</f>
         <v>0</v>
@@ -2711,7 +2719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <f>'Lojas Leves'!A11</f>
         <v>0</v>
@@ -2761,7 +2769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <f>'Lojas Leves'!A12</f>
         <v>0</v>
@@ -2811,7 +2819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <f>'Lojas Leves'!A13</f>
         <v>0</v>
@@ -2861,7 +2869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <f>'Lojas Leves'!A14</f>
         <v>0</v>
@@ -2911,7 +2919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <f>'Lojas Leves'!A15</f>
         <v>0</v>
@@ -2961,7 +2969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <f>'Lojas Leves'!A16</f>
         <v>0</v>
@@ -3011,7 +3019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <f>'Lojas Leves'!A17</f>
         <v>0</v>
@@ -3061,7 +3069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <f>'Lojas Leves'!A18</f>
         <v>0</v>
@@ -3111,7 +3119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <f>'Lojas Leves'!A19</f>
         <v>0</v>
@@ -3161,7 +3169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <f>'Lojas Leves'!A20</f>
         <v>0</v>
@@ -3211,45 +3219,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C21" s="15">
-        <f>SUM(C2:C20)</f>
+        <f t="shared" ref="C21:L21" si="1">SUM(C2:C20)</f>
         <v>450</v>
       </c>
       <c r="D21" s="15">
-        <f>SUM(D2:D20)</f>
+        <f t="shared" si="1"/>
         <v>2832.8665000000001</v>
       </c>
       <c r="E21" s="15">
-        <f>SUM(E2:E20)</f>
+        <f t="shared" si="1"/>
         <v>3507.5285999999996</v>
       </c>
       <c r="F21" s="15">
-        <f>SUM(F2:F20)</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="G21" s="15">
-        <f>SUM(G2:G20)</f>
+        <f t="shared" si="1"/>
         <v>118.8</v>
       </c>
       <c r="H21" s="15">
-        <f>SUM(H2:H20)</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="I21" s="15">
-        <f>SUM(I2:I20)</f>
+        <f t="shared" si="1"/>
         <v>47.4</v>
       </c>
       <c r="J21" s="15">
-        <f>SUM(J2:J20)</f>
+        <f t="shared" si="1"/>
         <v>2200</v>
       </c>
       <c r="K21" s="15">
-        <f>SUM(K2:K20)</f>
+        <f t="shared" si="1"/>
         <v>350</v>
       </c>
       <c r="L21" s="15">
-        <f>SUM(L2:L20)</f>
+        <f t="shared" si="1"/>
         <v>9626.5950999999986</v>
       </c>
     </row>
@@ -3263,19 +3271,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6CFD361-6156-4216-802A-7D34CA56C571}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A21" sqref="A21:XFD22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="15.77734375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="15.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3313,7 +3321,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <f>'Lojas Leves'!A2</f>
         <v>1</v>
@@ -3363,7 +3371,7 @@
         <v>4695.7256999999991</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <f>'Lojas Leves'!A3</f>
         <v>2</v>
@@ -3413,7 +3421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <f>'Lojas Leves'!A4</f>
         <v>3</v>
@@ -3463,7 +3471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <f>'Lojas Leves'!A5</f>
         <v>4</v>
@@ -3513,7 +3521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <f>'Lojas Leves'!A6</f>
         <v>0</v>
@@ -3563,7 +3571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <f>'Lojas Leves'!A7</f>
         <v>0</v>
@@ -3613,7 +3621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <f>'Lojas Leves'!A8</f>
         <v>0</v>
@@ -3663,7 +3671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <f>'Lojas Leves'!A9</f>
         <v>0</v>
@@ -3713,7 +3721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <f>'Lojas Leves'!A10</f>
         <v>0</v>
@@ -3763,7 +3771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <f>'Lojas Leves'!A11</f>
         <v>0</v>
@@ -3813,7 +3821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <f>'Lojas Leves'!A12</f>
         <v>0</v>
@@ -3863,7 +3871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <f>'Lojas Leves'!A13</f>
         <v>0</v>
@@ -3913,7 +3921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <f>'Lojas Leves'!A14</f>
         <v>0</v>
@@ -3963,7 +3971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <f>'Lojas Leves'!A15</f>
         <v>0</v>
@@ -4013,7 +4021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <f>'Lojas Leves'!A16</f>
         <v>0</v>
@@ -4063,7 +4071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <f>'Lojas Leves'!A17</f>
         <v>0</v>
@@ -4113,7 +4121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <f>'Lojas Leves'!A18</f>
         <v>0</v>
@@ -4163,7 +4171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <f>'Lojas Leves'!A19</f>
         <v>0</v>
@@ -4213,7 +4221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <f>'Lojas Leves'!A20</f>
         <v>0</v>
@@ -4263,45 +4271,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
-        <f>SUM(C2:C20)</f>
+        <f t="shared" ref="C21:L21" si="1">SUM(C2:C20)</f>
         <v>150</v>
       </c>
       <c r="D21" s="1">
-        <f>SUM(D2:D20)</f>
+        <f t="shared" si="1"/>
         <v>566.57330000000002</v>
       </c>
       <c r="E21" s="1">
-        <f>SUM(E2:E20)</f>
+        <f t="shared" si="1"/>
         <v>2338.3523999999998</v>
       </c>
       <c r="F21" s="1">
-        <f>SUM(F2:F20)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="G21" s="1">
-        <f>SUM(G2:G20)</f>
+        <f t="shared" si="1"/>
         <v>79.2</v>
       </c>
       <c r="H21" s="1">
-        <f>SUM(H2:H20)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="I21" s="1">
-        <f>SUM(I2:I20)</f>
+        <f t="shared" si="1"/>
         <v>31.6</v>
       </c>
       <c r="J21" s="1">
-        <f>SUM(J2:J20)</f>
+        <f t="shared" si="1"/>
         <v>1100</v>
       </c>
       <c r="K21" s="1">
-        <f>SUM(K2:K20)</f>
+        <f t="shared" si="1"/>
         <v>350</v>
       </c>
       <c r="L21" s="1">
-        <f>SUM(L2:L20)</f>
+        <f t="shared" si="1"/>
         <v>4695.7256999999991</v>
       </c>
     </row>

</xml_diff>